<commit_message>
WIP - Implementation charger parties
</commit_message>
<xml_diff>
--- a/documentation/Références.xlsx
+++ b/documentation/Références.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eliott.JAQUIER\MA20\BatailleNavale\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CPNV\BatailleNavale\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E21A5BD-CD7B-41FD-A930-813ACA7F89DB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5115" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide (Référence)" sheetId="2" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>https://www.tutorialspoint.com/how-to-clear-console-in-c</t>
   </si>
@@ -90,12 +91,15 @@
   </si>
   <si>
     <t>https://stackoverflow.com/questions/1442116/how-to-get-the-date-and-time-values-in-a-c-program</t>
+  </si>
+  <si>
+    <t>https://codes-sources.commentcamarche.net/source/53687-lister-fichiers-et-repertoires-multiplateforme</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -427,11 +431,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,29 +543,35 @@
         <v>19</v>
       </c>
     </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A11" r:id="rId10"/>
-    <hyperlink ref="A12" r:id="rId11"/>
-    <hyperlink ref="A13" r:id="rId12"/>
-    <hyperlink ref="A14" r:id="rId13"/>
-    <hyperlink ref="A15" r:id="rId14"/>
-    <hyperlink ref="A16" r:id="rId15"/>
-    <hyperlink ref="A17" r:id="rId16"/>
-    <hyperlink ref="A18" r:id="rId17"/>
-    <hyperlink ref="A19" r:id="rId18"/>
-    <hyperlink ref="A20" r:id="rId19"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="A14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="A15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="A17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="A18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="A19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="A20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="A21" r:id="rId20" xr:uid="{2C53690B-8DB6-413B-86B8-EF312E5333E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout de fonctions graphiques
</commit_message>
<xml_diff>
--- a/documentation/Références.xlsx
+++ b/documentation/Références.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CPNV\BatailleNavale\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E21A5BD-CD7B-41FD-A930-813ACA7F89DB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C843AD-5526-4E08-AAAD-6207DE447BFF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>https://www.tutorialspoint.com/how-to-clear-console-in-c</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>https://codes-sources.commentcamarche.net/source/53687-lister-fichiers-et-repertoires-multiplateforme</t>
+  </si>
+  <si>
+    <t>https://gist.github.com/mtancoigne/a51fe0686d51c05c6cd6ec5f42c856fc</t>
   </si>
 </sst>
 </file>
@@ -432,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
@@ -546,6 +549,11 @@
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Début d'un système de sons
</commit_message>
<xml_diff>
--- a/documentation/Références.xlsx
+++ b/documentation/Références.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CPNV\BatailleNavale\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C843AD-5526-4E08-AAAD-6207DE447BFF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4633BE95-E37C-4EA4-A192-7BD55E49E1E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>https://www.tutorialspoint.com/how-to-clear-console-in-c</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>https://gist.github.com/mtancoigne/a51fe0686d51c05c6cd6ec5f42c856fc</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/41421313/make-playsound-non-blocking</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,6 +557,11 @@
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -578,8 +586,9 @@
     <hyperlink ref="A19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="A20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
     <hyperlink ref="A21" r:id="rId20" xr:uid="{2C53690B-8DB6-413B-86B8-EF312E5333E3}"/>
+    <hyperlink ref="A23" r:id="rId21" xr:uid="{F0E96FFE-7D53-4756-8160-0491C5A462F5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajouts des animations en cours et fin de partie
</commit_message>
<xml_diff>
--- a/documentation/Références.xlsx
+++ b/documentation/Références.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CPNV\BatailleNavale\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3E485A-D626-4A32-8EAD-C5C952D94441}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865F401E-158F-4882-92B2-CE666E712586}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1515" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide (Référence)" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>https://www.tutorialspoint.com/how-to-clear-console-in-c</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>https://elifulkerson.com/projects/commandline-wav-player.php</t>
+  </si>
+  <si>
+    <t>Proposé par timothée rapin : https://codes-sources.commentcamarche.net/forum/affich-371867-plein-ecran-c-console donné</t>
   </si>
 </sst>
 </file>
@@ -441,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A28" sqref="A27:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,6 +573,11 @@
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -596,8 +604,9 @@
     <hyperlink ref="A21" r:id="rId20" xr:uid="{2C53690B-8DB6-413B-86B8-EF312E5333E3}"/>
     <hyperlink ref="A23" r:id="rId21" xr:uid="{F0E96FFE-7D53-4756-8160-0491C5A462F5}"/>
     <hyperlink ref="A24" r:id="rId22" xr:uid="{88CF4C2A-5041-4BA1-AE19-80E9B34D7409}"/>
+    <hyperlink ref="A25" r:id="rId23" display="https://codes-sources.commentcamarche.net/forum/affich-371867-plein-ecran-c-console donné par timothée rapin" xr:uid="{51FC6DF1-561D-46B5-93B1-9A12A7D51302}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>